<commit_message>
All volumes calculated but need values
</commit_message>
<xml_diff>
--- a/eerie_first_draft/PRIMAVERA_top_50.xlsx
+++ b/eerie_first_draft/PRIMAVERA_top_50.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\eerie\dreq\eerie_dreq\eerie_first_draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB80EF6F-1FC1-46E8-9E49-76E7E385D463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2FF739-95CF-47AD-9443-E75C24E7539B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -4223,8 +4223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4339,19 +4339,55 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
       <c r="E7">
         <f>1440*1920</f>
         <v>2764800</v>
       </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
       <c r="I7">
         <f>4322 * 3606</f>
         <v>15585132</v>
       </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
       <c r="M7">
         <v>85</v>
       </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
       <c r="Q7">
         <v>75</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
@@ -4427,96 +4463,150 @@
       <c r="B17" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="C17" s="6">
+        <f>SUM('6hrPlevPt'!$AC$2:$AC$100) / POWER(1024,3)</f>
+        <v>1.6996636986732483E-5</v>
+      </c>
+      <c r="D17" s="6">
+        <f>SUM('6hrPlevPt'!$AD$2:$AD$100) / POWER(1024,3)</f>
+        <v>3.3993273973464966E-5</v>
+      </c>
       <c r="E17" s="6">
         <f>SUM('6hrPlevPt'!$AE$2:$AE$100) / POWER(1024,3)</f>
         <v>46.992301940917969</v>
       </c>
-      <c r="F17" s="6"/>
+      <c r="F17" s="6">
+        <f>SUM('6hrPlevPt'!$AF$2:$AF$100) / POWER(1024,3)</f>
+        <v>5.0989910960197449E-5</v>
+      </c>
       <c r="G17" s="6">
         <f>SUM(C17:F17)</f>
-        <v>46.992301940917969</v>
+        <v>46.992403920739889</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>1022</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="C18" s="6">
+        <f>SUM(Prim6hr!$AC$2:$AC$100) / POWER(1024,3)</f>
+        <v>3.3993273973464966E-6</v>
+      </c>
+      <c r="D18" s="6">
+        <f>SUM(Prim6hr!$AD$2:$AD$100) / POWER(1024,3)</f>
+        <v>6.7986547946929932E-6</v>
+      </c>
       <c r="E18" s="6">
         <f>SUM(Prim6hr!$AE$2:$AE$100) / POWER(1024,3)</f>
         <v>9.3984603881835938</v>
       </c>
-      <c r="F18" s="6"/>
+      <c r="F18" s="6">
+        <f>SUM(Prim6hr!$AF$2:$AF$100) / POWER(1024,3)</f>
+        <v>1.019798219203949E-5</v>
+      </c>
       <c r="G18" s="6">
         <f t="shared" ref="G18:G22" si="0">SUM(C18:F18)</f>
-        <v>9.3984603881835938</v>
+        <v>9.3984807841479778</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="C19" s="6">
+        <f>SUM(Amon!$AC$2:$AC$100) / POWER(1024,3)</f>
+        <v>2.3720785975456238E-5</v>
+      </c>
+      <c r="D19" s="6">
+        <f>SUM(Amon!$AD$2:$AD$100) / POWER(1024,3)</f>
+        <v>4.7441571950912476E-5</v>
+      </c>
       <c r="E19" s="6">
         <f>SUM(Amon!$AE$2:$AE$100) / POWER(1024,3)</f>
-        <v>70.681571960449219</v>
-      </c>
-      <c r="F19" s="6"/>
+        <v>65.583229064941406</v>
+      </c>
+      <c r="F19" s="6">
+        <f>SUM(Amon!$AF$2:$AF$100) / POWER(1024,3)</f>
+        <v>7.1162357926368713E-5</v>
+      </c>
       <c r="G19" s="6">
         <f t="shared" si="0"/>
-        <v>70.681571960449219</v>
+        <v>65.583371389657259</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="C20" s="6">
+        <f>SUM(Oday!$AC$2:$AC$100) / POWER(1024,3)</f>
+        <v>2.5494955480098724E-6</v>
+      </c>
+      <c r="D20" s="6">
+        <f>SUM(Oday!$AD$2:$AD$100) / POWER(1024,3)</f>
+        <v>5.0989910960197449E-6</v>
+      </c>
       <c r="E20" s="6">
         <f>SUM(Oday!$AE$2:$AE$100) / POWER(1024,3)</f>
-        <v>158.9368985965848</v>
-      </c>
-      <c r="F20" s="6"/>
+        <v>39.734224649146199</v>
+      </c>
+      <c r="F20" s="6">
+        <f>SUM(Oday!$AF$2:$AF$100) / POWER(1024,3)</f>
+        <v>7.6484866440296173E-6</v>
+      </c>
       <c r="G20" s="6">
         <f t="shared" si="0"/>
-        <v>158.9368985965848</v>
+        <v>39.734239946119487</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+      <c r="C21" s="6">
+        <f>SUM(SIday!$AC$2:$AC$100) / POWER(1024,3)</f>
+        <v>3.3993273973464966E-6</v>
+      </c>
+      <c r="D21" s="6">
+        <f>SUM(SIday!$AD$2:$AD$100) / POWER(1024,3)</f>
+        <v>6.7986547946929932E-6</v>
+      </c>
       <c r="E21" s="6">
         <f>SUM(SIday!$AE$2:$AE$100) / POWER(1024,3)</f>
-        <v>211.9158647954464</v>
-      </c>
-      <c r="F21" s="6"/>
+        <v>52.978966198861599</v>
+      </c>
+      <c r="F21" s="6">
+        <f>SUM(SIday!$AF$2:$AF$100) / POWER(1024,3)</f>
+        <v>1.019798219203949E-5</v>
+      </c>
       <c r="G21" s="6">
         <f t="shared" si="0"/>
-        <v>211.9158647954464</v>
+        <v>52.978986594825983</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
+      <c r="C22" s="6">
+        <f>SUM(day!$AC$2:$AC$100) / POWER(1024,3)</f>
+        <v>7.2235707193613052E-5</v>
+      </c>
+      <c r="D22" s="6">
+        <f>SUM(day!$AD$2:$AD$100) / POWER(1024,3)</f>
+        <v>1.444714143872261E-4</v>
+      </c>
       <c r="E22" s="6">
         <f>SUM(day!$AE$2:$AE$100) / POWER(1024,3)</f>
-        <v>798.86913299560547</v>
-      </c>
-      <c r="F22" s="6"/>
+        <v>199.71728324890137</v>
+      </c>
+      <c r="F22" s="6">
+        <f>SUM(day!$AF$2:$AF$100) / POWER(1024,3)</f>
+        <v>2.1670712158083916E-4</v>
+      </c>
       <c r="G22" s="6">
         <f t="shared" si="0"/>
-        <v>798.86913299560547</v>
+        <v>199.71771666314453</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
@@ -4567,23 +4657,23 @@
       </c>
       <c r="C29" s="6">
         <f>SUM(C17:C28)</f>
-        <v>0</v>
+        <v>1.2230128049850464E-4</v>
       </c>
       <c r="D29" s="6">
         <f t="shared" ref="D29:G29" si="1">SUM(D17:D28)</f>
-        <v>0</v>
+        <v>2.4460256099700928E-4</v>
       </c>
       <c r="E29" s="6">
         <f t="shared" si="1"/>
-        <v>1296.7942306771874</v>
+        <v>414.40446549095213</v>
       </c>
       <c r="F29" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.6690384149551392E-4</v>
       </c>
       <c r="G29" s="6">
         <f t="shared" si="1"/>
-        <v>1296.7942306771874</v>
+        <v>414.40519929863513</v>
       </c>
     </row>
   </sheetData>
@@ -4605,7 +4695,7 @@
   <dimension ref="A1:AF6"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="M1" activeCellId="15" sqref="AB1:AB1048576 AA1:AA1048576 Z1:Z1048576 Y1:Y1048576 X1:X1048576 W1:W1048576 V1:V1048576 U1:U1048576 T1:T1048576 S1:S1048576 R1:R1048576 Q1:Q1048576 P1:P1048576 O1:O1048576 N1:N1048576 M1:M1048576"/>
+      <selection activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4784,9 +4874,21 @@
       <c r="AB2" s="2" t="s">
         <v>242</v>
       </c>
+      <c r="AC2">
+        <f>Notes!$C$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>3650</v>
+      </c>
+      <c r="AD2">
+        <f>Notes!$D$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>7300</v>
+      </c>
       <c r="AE2">
         <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
         <v>10091520000</v>
+      </c>
+      <c r="AF2">
+        <f>Notes!$F$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>10950</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="129.6" x14ac:dyDescent="0.3">
@@ -4860,9 +4962,21 @@
       <c r="AB3" s="2" t="s">
         <v>247</v>
       </c>
+      <c r="AC3">
+        <f>Notes!$C$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>3650</v>
+      </c>
+      <c r="AD3">
+        <f>Notes!$D$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>7300</v>
+      </c>
       <c r="AE3">
         <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
         <v>10091520000</v>
+      </c>
+      <c r="AF3">
+        <f>Notes!$F$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>10950</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -4938,9 +5052,21 @@
       <c r="AB4" s="2" t="s">
         <v>221</v>
       </c>
+      <c r="AC4">
+        <f>Notes!$C$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>3650</v>
+      </c>
+      <c r="AD4">
+        <f>Notes!$D$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>7300</v>
+      </c>
       <c r="AE4">
         <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
         <v>10091520000</v>
+      </c>
+      <c r="AF4">
+        <f>Notes!$F$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>10950</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -5016,9 +5142,21 @@
       <c r="AB5" s="2" t="s">
         <v>221</v>
       </c>
+      <c r="AC5">
+        <f>Notes!$C$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>3650</v>
+      </c>
+      <c r="AD5">
+        <f>Notes!$D$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>7300</v>
+      </c>
       <c r="AE5">
         <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
         <v>10091520000</v>
+      </c>
+      <c r="AF5">
+        <f>Notes!$F$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>10950</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -5092,9 +5230,21 @@
       <c r="AB6" s="2" t="s">
         <v>221</v>
       </c>
+      <c r="AC6">
+        <f>Notes!$C$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>3650</v>
+      </c>
+      <c r="AD6">
+        <f>Notes!$D$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>7300</v>
+      </c>
       <c r="AE6">
         <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
         <v>10091520000</v>
+      </c>
+      <c r="AF6">
+        <f>Notes!$F$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>10950</v>
       </c>
     </row>
   </sheetData>
@@ -5275,9 +5425,21 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
       <c r="AB2" s="2"/>
+      <c r="AC2">
+        <f>Notes!$C$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>3650</v>
+      </c>
+      <c r="AD2">
+        <f>Notes!$D$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>7300</v>
+      </c>
       <c r="AE2">
         <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
         <v>10091520000</v>
+      </c>
+      <c r="AF2">
+        <f>Notes!$F$7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>10950</v>
       </c>
     </row>
   </sheetData>
@@ -5291,7 +5453,7 @@
   <dimension ref="A1:AF76"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AE75" sqref="AE75:AE76"/>
+      <selection activeCell="AE5" sqref="AE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5483,9 +5645,21 @@
       <c r="AB2" s="2" t="s">
         <v>294</v>
       </c>
+      <c r="AC2">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD2">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE2">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
+      </c>
+      <c r="AF2">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
@@ -5571,9 +5745,21 @@
       <c r="AB3" s="2" t="s">
         <v>298</v>
       </c>
+      <c r="AC3">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD3">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE3">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
+      </c>
+      <c r="AF3">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
@@ -5659,9 +5845,21 @@
       <c r="AB4" s="2" t="s">
         <v>298</v>
       </c>
+      <c r="AC4">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD4">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE4">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
+      </c>
+      <c r="AF4">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
@@ -5747,9 +5945,21 @@
       <c r="AB5" s="2" t="s">
         <v>298</v>
       </c>
+      <c r="AC5">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD5">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE5">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
+      </c>
+      <c r="AF5">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
@@ -5835,9 +6045,21 @@
       <c r="AB6" s="2" t="s">
         <v>331</v>
       </c>
+      <c r="AC6">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD6">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE6">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
+      </c>
+      <c r="AF6">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -5923,9 +6145,21 @@
       <c r="AB7" s="2" t="s">
         <v>338</v>
       </c>
+      <c r="AC7">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD7">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE7">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
+      </c>
+      <c r="AF7">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
@@ -6009,9 +6243,21 @@
       <c r="AB8" s="2" t="s">
         <v>346</v>
       </c>
+      <c r="AC8">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD8">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE8">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
+      </c>
+      <c r="AF8">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
@@ -6095,9 +6341,21 @@
       <c r="AB9" s="2" t="s">
         <v>294</v>
       </c>
+      <c r="AC9">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD9">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE9">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
+      </c>
+      <c r="AF9">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
@@ -6183,9 +6441,21 @@
       <c r="AB10" s="2" t="s">
         <v>298</v>
       </c>
+      <c r="AC10">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD10">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE10">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
+      </c>
+      <c r="AF10">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -6271,9 +6541,21 @@
       <c r="AB11" s="2" t="s">
         <v>361</v>
       </c>
+      <c r="AC11">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD11">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE11">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
+      </c>
+      <c r="AF11">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
@@ -6357,9 +6639,21 @@
       <c r="AB12" s="2" t="s">
         <v>298</v>
       </c>
+      <c r="AC12">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD12">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE12">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
+      </c>
+      <c r="AF12">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
@@ -6445,9 +6739,21 @@
       <c r="AB13" s="2" t="s">
         <v>294</v>
       </c>
+      <c r="AC13">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD13">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE13">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
+      </c>
+      <c r="AF13">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
@@ -6533,9 +6839,21 @@
       <c r="AB14" s="2" t="s">
         <v>298</v>
       </c>
+      <c r="AC14">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD14">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE14">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
+      </c>
+      <c r="AF14">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -6621,9 +6939,21 @@
       <c r="AB15" s="2" t="s">
         <v>361</v>
       </c>
+      <c r="AC15">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD15">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE15">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
+      </c>
+      <c r="AF15">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:32" ht="72" x14ac:dyDescent="0.3">
@@ -6701,12 +7031,24 @@
       <c r="AB16" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="AC16">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD16">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE16">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF16">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="17" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
@@ -6789,12 +7131,24 @@
       <c r="AB17" s="2" t="s">
         <v>399</v>
       </c>
+      <c r="AC17">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD17">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE17">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF17">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="18" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
@@ -6877,12 +7231,24 @@
       <c r="AB18" s="2" t="s">
         <v>338</v>
       </c>
+      <c r="AC18">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD18">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE18">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF18">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="19" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
@@ -6965,12 +7331,24 @@
       <c r="AB19" s="2" t="s">
         <v>338</v>
       </c>
+      <c r="AC19">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD19">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE19">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF19">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="20" spans="1:31" ht="144" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" ht="144" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -7054,13 +7432,25 @@
       </c>
       <c r="AB20" s="2" t="s">
         <v>387</v>
+      </c>
+      <c r="AC20">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD20">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
       </c>
       <c r="AE20">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF20">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="21" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
@@ -7143,12 +7533,24 @@
       <c r="AB21" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="AC21">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD21">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE21">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF21">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="22" spans="1:31" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
@@ -7231,12 +7633,24 @@
       <c r="AB22" s="2" t="s">
         <v>298</v>
       </c>
+      <c r="AC22">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD22">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE22">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF22">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="23" spans="1:31" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
@@ -7319,12 +7733,24 @@
       <c r="AB23" s="2" t="s">
         <v>361</v>
       </c>
+      <c r="AC23">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD23">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE23">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF23">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="24" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>38</v>
       </c>
@@ -7407,12 +7833,24 @@
       <c r="AB24" s="2" t="s">
         <v>298</v>
       </c>
+      <c r="AC24">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD24">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE24">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF24">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="25" spans="1:31" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:32" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
@@ -7495,12 +7933,24 @@
       <c r="AB25" s="2" t="s">
         <v>361</v>
       </c>
+      <c r="AC25">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD25">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE25">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF25">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="26" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -7575,12 +8025,24 @@
       <c r="AB26" s="2" t="s">
         <v>361</v>
       </c>
+      <c r="AC26">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD26">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE26">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF26">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="27" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>38</v>
       </c>
@@ -7663,12 +8125,24 @@
       <c r="AB27" s="2" t="s">
         <v>361</v>
       </c>
+      <c r="AC27">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD27">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE27">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF27">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="28" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
@@ -7751,12 +8225,24 @@
       <c r="AB28" s="2" t="s">
         <v>361</v>
       </c>
+      <c r="AC28">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD28">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE28">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF28">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="29" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
@@ -7840,13 +8326,25 @@
       </c>
       <c r="AB29" s="2" t="s">
         <v>387</v>
+      </c>
+      <c r="AC29">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD29">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
       </c>
       <c r="AE29">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF29">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="30" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
@@ -7929,12 +8427,24 @@
       <c r="AB30" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="AC30">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD30">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE30">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF30">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="31" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
@@ -8017,12 +8527,24 @@
       <c r="AB31" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="AC31">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD31">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE31">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF31">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="32" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
@@ -8105,12 +8627,24 @@
       <c r="AB32" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="AC32">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD32">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE32">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF32">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="33" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -8193,12 +8727,24 @@
       <c r="AB33" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="AC33">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD33">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE33">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF33">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="34" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -8279,12 +8825,24 @@
       <c r="AB34" s="2" t="s">
         <v>361</v>
       </c>
+      <c r="AC34">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD34">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE34">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF34">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="35" spans="1:31" ht="72" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:32" ht="72" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>38</v>
       </c>
@@ -8367,12 +8925,24 @@
       <c r="AB35" s="2" t="s">
         <v>298</v>
       </c>
+      <c r="AC35">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD35">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE35">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF35">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="36" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:32" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
@@ -8453,12 +9023,24 @@
       <c r="AB36" s="2" t="s">
         <v>399</v>
       </c>
+      <c r="AC36">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD36">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE36">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF36">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="37" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:32" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>38</v>
       </c>
@@ -8537,12 +9119,24 @@
       <c r="AB37" s="2" t="s">
         <v>399</v>
       </c>
+      <c r="AC37">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD37">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE37">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF37">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="38" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:32" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
@@ -8626,13 +9220,25 @@
       </c>
       <c r="AB38" s="2" t="s">
         <v>538</v>
+      </c>
+      <c r="AC38">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD38">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
       </c>
       <c r="AE38">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF38">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="39" spans="1:31" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:32" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -8713,12 +9319,24 @@
       <c r="AB39" s="2" t="s">
         <v>549</v>
       </c>
+      <c r="AC39">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD39">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE39">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF39">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="40" spans="1:31" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:32" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -8799,12 +9417,24 @@
       <c r="AB40" s="2" t="s">
         <v>549</v>
       </c>
+      <c r="AC40">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD40">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE40">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF40">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="41" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>38</v>
       </c>
@@ -8887,12 +9517,24 @@
       <c r="AB41" s="2" t="s">
         <v>361</v>
       </c>
+      <c r="AC41">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD41">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE41">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF41">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="42" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>38</v>
       </c>
@@ -8973,12 +9615,24 @@
       <c r="AB42" s="2" t="s">
         <v>577</v>
       </c>
+      <c r="AC42">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD42">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE42">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF42">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="43" spans="1:31" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:32" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>38</v>
       </c>
@@ -9059,12 +9713,24 @@
       <c r="AB43" s="2" t="s">
         <v>589</v>
       </c>
+      <c r="AC43">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD43">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE43">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF43">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="44" spans="1:31" ht="72" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:32" ht="72" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>38</v>
       </c>
@@ -9137,12 +9803,24 @@
       <c r="AB44" s="2" t="s">
         <v>589</v>
       </c>
+      <c r="AC44">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD44">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE44">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF44">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="45" spans="1:31" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:32" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>38</v>
       </c>
@@ -9225,12 +9903,24 @@
       <c r="AB45" s="2" t="s">
         <v>589</v>
       </c>
+      <c r="AC45">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD45">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE45">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF45">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="46" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>38</v>
       </c>
@@ -9311,12 +10001,24 @@
       <c r="AB46" s="2" t="s">
         <v>620</v>
       </c>
+      <c r="AC46">
+        <f>Notes!$C$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>2550</v>
+      </c>
+      <c r="AD46">
+        <f>Notes!$D$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>5100</v>
+      </c>
       <c r="AE46">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>7050240000</v>
       </c>
+      <c r="AF46">
+        <f>Notes!$F$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>7650</v>
+      </c>
     </row>
-    <row r="47" spans="1:31" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:32" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>38</v>
       </c>
@@ -9391,12 +10093,24 @@
       <c r="AB47" s="2" t="s">
         <v>630</v>
       </c>
+      <c r="AC47">
+        <f>Notes!$C$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>2550</v>
+      </c>
+      <c r="AD47">
+        <f>Notes!$D$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>5100</v>
+      </c>
       <c r="AE47">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>7050240000</v>
       </c>
+      <c r="AF47">
+        <f>Notes!$F$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>7650</v>
+      </c>
     </row>
-    <row r="48" spans="1:31" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:32" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>38</v>
       </c>
@@ -9471,12 +10185,24 @@
       <c r="AB48" s="2" t="s">
         <v>639</v>
       </c>
+      <c r="AC48">
+        <f>Notes!$C$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>2550</v>
+      </c>
+      <c r="AD48">
+        <f>Notes!$D$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>5100</v>
+      </c>
       <c r="AE48">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>7050240000</v>
       </c>
+      <c r="AF48">
+        <f>Notes!$F$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>7650</v>
+      </c>
     </row>
-    <row r="49" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>38</v>
       </c>
@@ -9551,12 +10277,24 @@
       <c r="AB49" s="2" t="s">
         <v>639</v>
       </c>
+      <c r="AC49">
+        <f>Notes!$C$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>2550</v>
+      </c>
+      <c r="AD49">
+        <f>Notes!$D$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>5100</v>
+      </c>
       <c r="AE49">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>7050240000</v>
       </c>
+      <c r="AF49">
+        <f>Notes!$F$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>7650</v>
+      </c>
     </row>
-    <row r="50" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>38</v>
       </c>
@@ -9637,12 +10375,24 @@
       <c r="AB50" s="2" t="s">
         <v>660</v>
       </c>
+      <c r="AC50">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD50">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE50">
-        <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>7050240000</v>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1575936000</v>
+      </c>
+      <c r="AF50">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
       </c>
     </row>
-    <row r="51" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>38</v>
       </c>
@@ -9723,12 +10473,24 @@
       <c r="AB51" s="2" t="s">
         <v>660</v>
       </c>
+      <c r="AC51">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD51">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE51">
-        <f>Notes!$E$7 *19 * Notes!$C$10 * Notes!$C$13</f>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
         <v>1575936000</v>
       </c>
+      <c r="AF51">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
+      </c>
     </row>
-    <row r="52" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>38</v>
       </c>
@@ -9809,12 +10571,24 @@
       <c r="AB52" s="2" t="s">
         <v>660</v>
       </c>
+      <c r="AC52">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD52">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE52">
-        <f>Notes!$E$7 *19 * Notes!$C$10 * Notes!$C$13</f>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
         <v>1575936000</v>
       </c>
+      <c r="AF52">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
+      </c>
     </row>
-    <row r="53" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>38</v>
       </c>
@@ -9893,12 +10667,24 @@
       <c r="AB53" s="2" t="s">
         <v>331</v>
       </c>
+      <c r="AC53">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD53">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE53">
-        <f>Notes!$E$7 *19 * Notes!$C$10 * Notes!$C$13</f>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
         <v>1575936000</v>
       </c>
+      <c r="AF53">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
+      </c>
     </row>
-    <row r="54" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>38</v>
       </c>
@@ -9981,12 +10767,24 @@
       <c r="AB54" s="2" t="s">
         <v>620</v>
       </c>
+      <c r="AC54">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD54">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE54">
-        <f>Notes!$E$7 *19 * Notes!$C$10 * Notes!$C$13</f>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
         <v>1575936000</v>
       </c>
+      <c r="AF54">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
+      </c>
     </row>
-    <row r="55" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>38</v>
       </c>
@@ -10067,12 +10865,24 @@
       <c r="AB55" s="2" t="s">
         <v>660</v>
       </c>
+      <c r="AC55">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD55">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE55">
-        <f>Notes!$E$7 *19 * Notes!$C$10 * Notes!$C$13</f>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
         <v>1575936000</v>
       </c>
+      <c r="AF55">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
+      </c>
     </row>
-    <row r="56" spans="1:31" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:32" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>38</v>
       </c>
@@ -10151,12 +10961,24 @@
       <c r="AB56" s="2" t="s">
         <v>660</v>
       </c>
+      <c r="AC56">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD56">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE56">
-        <f>Notes!$E$7 *19 * Notes!$C$10 * Notes!$C$13</f>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
         <v>1575936000</v>
       </c>
+      <c r="AF56">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
+      </c>
     </row>
-    <row r="57" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>38</v>
       </c>
@@ -10229,12 +11051,24 @@
       <c r="AB57" s="2" t="s">
         <v>549</v>
       </c>
+      <c r="AC57">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD57">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE57">
-        <f>Notes!$E$7 *19 * Notes!$C$10 * Notes!$C$13</f>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
         <v>1575936000</v>
       </c>
+      <c r="AF57">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
+      </c>
     </row>
-    <row r="58" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>38</v>
       </c>
@@ -10307,12 +11141,24 @@
       <c r="AB58" s="2" t="s">
         <v>549</v>
       </c>
+      <c r="AC58">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD58">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE58">
-        <f>Notes!$E$7 *19 * Notes!$C$10 * Notes!$C$13</f>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
         <v>1575936000</v>
       </c>
+      <c r="AF58">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
+      </c>
     </row>
-    <row r="59" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>38</v>
       </c>
@@ -10385,12 +11231,24 @@
       <c r="AB59" s="2" t="s">
         <v>718</v>
       </c>
+      <c r="AC59">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD59">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE59">
-        <f>Notes!$E$7 *19 * Notes!$C$10 * Notes!$C$13</f>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
         <v>1575936000</v>
       </c>
+      <c r="AF59">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
+      </c>
     </row>
-    <row r="60" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>38</v>
       </c>
@@ -10463,12 +11321,24 @@
       <c r="AB60" s="2" t="s">
         <v>718</v>
       </c>
+      <c r="AC60">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD60">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE60">
-        <f>Notes!$E$7 *19 * Notes!$C$10 * Notes!$C$13</f>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
         <v>1575936000</v>
       </c>
+      <c r="AF60">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
+      </c>
     </row>
-    <row r="61" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>38</v>
       </c>
@@ -10539,12 +11409,24 @@
       <c r="AB61" s="2" t="s">
         <v>733</v>
       </c>
+      <c r="AC61">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD61">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE61">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF61">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="62" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>38</v>
       </c>
@@ -10615,12 +11497,24 @@
       <c r="AB62" s="2" t="s">
         <v>718</v>
       </c>
+      <c r="AC62">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD62">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE62">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF62">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="63" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>38</v>
       </c>
@@ -10693,12 +11587,24 @@
       <c r="AB63" s="2" t="s">
         <v>718</v>
       </c>
+      <c r="AC63">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD63">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE63">
-        <f>Notes!$E$7 *19 * Notes!$C$10 * Notes!$C$13</f>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
         <v>1575936000</v>
       </c>
+      <c r="AF63">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
+      </c>
     </row>
-    <row r="64" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>38</v>
       </c>
@@ -10771,12 +11677,24 @@
       <c r="AB64" s="2" t="s">
         <v>718</v>
       </c>
+      <c r="AC64">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD64">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE64">
-        <f>Notes!$E$7 *19 * Notes!$C$10 * Notes!$C$13</f>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
         <v>1575936000</v>
       </c>
+      <c r="AF64">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
+      </c>
     </row>
-    <row r="65" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>38</v>
       </c>
@@ -10847,12 +11765,24 @@
       <c r="AB65" s="2" t="s">
         <v>718</v>
       </c>
+      <c r="AC65">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD65">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE65">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF65">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="66" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>38</v>
       </c>
@@ -10923,12 +11853,24 @@
       <c r="AB66" s="2" t="s">
         <v>718</v>
       </c>
+      <c r="AC66">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD66">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE66">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF66">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="67" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>38</v>
       </c>
@@ -11001,12 +11943,24 @@
       <c r="AB67" s="2" t="s">
         <v>718</v>
       </c>
+      <c r="AC67">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD67">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE67">
-        <f>Notes!$E$7 *19 * Notes!$C$10 * Notes!$C$13</f>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
         <v>1575936000</v>
       </c>
+      <c r="AF67">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
+      </c>
     </row>
-    <row r="68" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>38</v>
       </c>
@@ -11079,12 +12033,24 @@
       <c r="AB68" s="2" t="s">
         <v>718</v>
       </c>
+      <c r="AC68">
+        <f>Notes!$C$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>570</v>
+      </c>
+      <c r="AD68">
+        <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1140</v>
+      </c>
       <c r="AE68">
-        <f>Notes!$E$7 *19 * Notes!$C$10 * Notes!$C$13</f>
+        <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
         <v>1575936000</v>
       </c>
+      <c r="AF68">
+        <f>Notes!$F$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
+        <v>1710</v>
+      </c>
     </row>
-    <row r="69" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>38</v>
       </c>
@@ -11155,12 +12121,24 @@
       <c r="AB69" s="2" t="s">
         <v>718</v>
       </c>
+      <c r="AC69">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD69">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE69">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF69">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="70" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>38</v>
       </c>
@@ -11231,12 +12209,24 @@
       <c r="AB70" s="2" t="s">
         <v>718</v>
       </c>
+      <c r="AC70">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD70">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE70">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF70">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="71" spans="1:31" ht="72" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:32" ht="72" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>259</v>
       </c>
@@ -11307,12 +12297,24 @@
       <c r="AB71" s="2" t="s">
         <v>785</v>
       </c>
+      <c r="AC71">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD71">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE71">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF71">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="72" spans="1:31" ht="72" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:32" ht="72" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>259</v>
       </c>
@@ -11383,12 +12385,24 @@
       <c r="AB72" s="2" t="s">
         <v>785</v>
       </c>
+      <c r="AC72">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD72">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE72">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF72">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="73" spans="1:31" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:32" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>259</v>
       </c>
@@ -11459,12 +12473,24 @@
       <c r="AB73" s="2" t="s">
         <v>785</v>
       </c>
+      <c r="AC73">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD73">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE73">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF73">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="74" spans="1:31" ht="72" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:32" ht="72" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>259</v>
       </c>
@@ -11535,12 +12561,24 @@
       <c r="AB74" s="2" t="s">
         <v>785</v>
       </c>
+      <c r="AC74">
+        <f>Notes!$C$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>30</v>
+      </c>
+      <c r="AD74">
+        <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
+      </c>
       <c r="AE74">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>82944000</v>
       </c>
+      <c r="AF74">
+        <f>Notes!$F$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>90</v>
+      </c>
     </row>
-    <row r="75" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>38</v>
       </c>
@@ -11613,12 +12651,24 @@
       <c r="AB75" s="2" t="s">
         <v>639</v>
       </c>
+      <c r="AC75">
+        <f>Notes!$C$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>2550</v>
+      </c>
+      <c r="AD75">
+        <f>Notes!$D$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>5100</v>
+      </c>
       <c r="AE75">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>7050240000</v>
       </c>
+      <c r="AF75">
+        <f>Notes!$F$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>7650</v>
+      </c>
     </row>
-    <row r="76" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>38</v>
       </c>
@@ -11691,9 +12741,21 @@
       <c r="AB76" s="2" t="s">
         <v>639</v>
       </c>
+      <c r="AC76">
+        <f>Notes!$C$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>2550</v>
+      </c>
+      <c r="AD76">
+        <f>Notes!$D$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>5100</v>
+      </c>
       <c r="AE76">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>7050240000</v>
+      </c>
+      <c r="AF76">
+        <f>Notes!$F$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>7650</v>
       </c>
     </row>
   </sheetData>
@@ -11706,8 +12768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2:AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11888,9 +12950,21 @@
       <c r="AB2" s="2" t="s">
         <v>854</v>
       </c>
+      <c r="AC2">
+        <f>Notes!$G$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD2">
+        <f>Notes!$H$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE2">
-        <f>Notes!$I$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>56885731800</v>
+        <f>Notes!$I$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>14221432950</v>
+      </c>
+      <c r="AF2">
+        <f>Notes!$J$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="100.8" x14ac:dyDescent="0.3">
@@ -11966,9 +13040,21 @@
       <c r="AB3" s="2" t="s">
         <v>857</v>
       </c>
+      <c r="AC3">
+        <f>Notes!$G$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD3">
+        <f>Notes!$H$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE3">
-        <f>Notes!$I$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>56885731800</v>
+        <f>Notes!$I$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>14221432950</v>
+      </c>
+      <c r="AF3">
+        <f>Notes!$J$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="86.4" x14ac:dyDescent="0.3">
@@ -12044,9 +13130,21 @@
       <c r="AB4" s="2" t="s">
         <v>869</v>
       </c>
+      <c r="AC4">
+        <f>Notes!$G$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD4">
+        <f>Notes!$H$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE4">
-        <f>Notes!$I$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>56885731800</v>
+        <f>Notes!$I$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>14221432950</v>
+      </c>
+      <c r="AF4">
+        <f>Notes!$J$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
   </sheetData>
@@ -12060,7 +13158,7 @@
   <dimension ref="A1:AF5"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AE3" sqref="AE3:AE5"/>
+      <selection activeCell="AD9" sqref="AD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12247,9 +13345,21 @@
       <c r="AB2" s="2" t="s">
         <v>882</v>
       </c>
+      <c r="AC2">
+        <f>Notes!$G$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD2">
+        <f>Notes!$H$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE2">
-        <f>Notes!$I$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>56885731800</v>
+        <f>Notes!$I$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>14221432950</v>
+      </c>
+      <c r="AF2">
+        <f>Notes!$J$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
@@ -12331,9 +13441,21 @@
       <c r="AB3" s="2" t="s">
         <v>895</v>
       </c>
+      <c r="AC3">
+        <f>Notes!$G$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD3">
+        <f>Notes!$H$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE3">
-        <f>Notes!$I$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>56885731800</v>
+        <f>Notes!$I$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>14221432950</v>
+      </c>
+      <c r="AF3">
+        <f>Notes!$J$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -12407,9 +13529,21 @@
       <c r="AB4" s="2" t="s">
         <v>905</v>
       </c>
+      <c r="AC4">
+        <f>Notes!$G$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD4">
+        <f>Notes!$H$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE4">
-        <f>Notes!$I$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>56885731800</v>
+        <f>Notes!$I$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>14221432950</v>
+      </c>
+      <c r="AF4">
+        <f>Notes!$J$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -12483,9 +13617,21 @@
       <c r="AB5" s="2" t="s">
         <v>905</v>
       </c>
+      <c r="AC5">
+        <f>Notes!$G$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD5">
+        <f>Notes!$H$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE5">
-        <f>Notes!$I$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>56885731800</v>
+        <f>Notes!$I$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>14221432950</v>
+      </c>
+      <c r="AF5">
+        <f>Notes!$J$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
   </sheetData>
@@ -12498,8 +13644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView topLeftCell="I28" workbookViewId="0">
-      <selection activeCell="AE32" sqref="AE32:AE37"/>
+    <sheetView topLeftCell="I31" workbookViewId="0">
+      <selection activeCell="AC37" sqref="AC37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12680,9 +13826,21 @@
       <c r="AB2" s="2" t="s">
         <v>914</v>
       </c>
+      <c r="AC2">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD2">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE2">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF2">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -12758,9 +13916,21 @@
       <c r="AB3" s="2" t="s">
         <v>919</v>
       </c>
+      <c r="AC3">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD3">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE3">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF3">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -12836,9 +14006,21 @@
       <c r="AB4" s="2" t="s">
         <v>919</v>
       </c>
+      <c r="AC4">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD4">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE4">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF4">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -12914,9 +14096,21 @@
       <c r="AB5" s="2" t="s">
         <v>924</v>
       </c>
+      <c r="AC5">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD5">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE5">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF5">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="6" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
@@ -12994,9 +14188,21 @@
       <c r="AB6" s="2" t="s">
         <v>926</v>
       </c>
+      <c r="AC6">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD6">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE6">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF6">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="7" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -13072,9 +14278,21 @@
       <c r="AB7" s="2" t="s">
         <v>928</v>
       </c>
+      <c r="AC7">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD7">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE7">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF7">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="8" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
@@ -13150,9 +14368,21 @@
       <c r="AB8" s="2" t="s">
         <v>930</v>
       </c>
+      <c r="AC8">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD8">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE8">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF8">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="9" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
@@ -13228,9 +14458,21 @@
       <c r="AB9" s="2" t="s">
         <v>932</v>
       </c>
+      <c r="AC9">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD9">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE9">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF9">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="10" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
@@ -13308,9 +14550,21 @@
       <c r="AB10" s="2" t="s">
         <v>934</v>
       </c>
+      <c r="AC10">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD10">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE10">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF10">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="11" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -13388,9 +14642,21 @@
       <c r="AB11" s="2" t="s">
         <v>936</v>
       </c>
+      <c r="AC11">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD11">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE11">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF11">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="12" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -13468,9 +14734,21 @@
       <c r="AB12" s="2" t="s">
         <v>941</v>
       </c>
+      <c r="AC12">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD12">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE12">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF12">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="13" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -13548,9 +14826,21 @@
       <c r="AB13" s="2" t="s">
         <v>947</v>
       </c>
+      <c r="AC13">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD13">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE13">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF13">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="14" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
@@ -13626,9 +14916,21 @@
       <c r="AB14" s="2" t="s">
         <v>949</v>
       </c>
+      <c r="AC14">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD14">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE14">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF14">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="15" spans="1:32" ht="72" x14ac:dyDescent="0.3">
@@ -13714,9 +15016,21 @@
       <c r="AB15" s="2" t="s">
         <v>952</v>
       </c>
+      <c r="AC15">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD15">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE15">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF15">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
     <row r="16" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
@@ -13792,12 +15106,24 @@
       <c r="AB16" s="2" t="s">
         <v>957</v>
       </c>
+      <c r="AC16">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD16">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE16">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF16">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="17" spans="1:31" ht="72" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" ht="72" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
@@ -13872,12 +15198,24 @@
       <c r="AB17" s="2" t="s">
         <v>949</v>
       </c>
+      <c r="AC17">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD17">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE17">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF17">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="18" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
@@ -13952,12 +15290,24 @@
       <c r="AB18" s="2" t="s">
         <v>961</v>
       </c>
+      <c r="AC18">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD18">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE18">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF18">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="19" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
@@ -14032,12 +15382,24 @@
       <c r="AB19" s="2" t="s">
         <v>963</v>
       </c>
+      <c r="AC19">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD19">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE19">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF19">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="20" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -14112,12 +15474,24 @@
       <c r="AB20" s="2" t="s">
         <v>949</v>
       </c>
+      <c r="AC20">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD20">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE20">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF20">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="21" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>38</v>
       </c>
@@ -14190,12 +15564,24 @@
       <c r="AB21" s="2" t="s">
         <v>967</v>
       </c>
+      <c r="AC21">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD21">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE21">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF21">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="22" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
@@ -14268,12 +15654,24 @@
       <c r="AB22" s="2" t="s">
         <v>967</v>
       </c>
+      <c r="AC22">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD22">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE22">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF22">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="23" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
@@ -14346,12 +15744,24 @@
       <c r="AB23" s="2" t="s">
         <v>976</v>
       </c>
+      <c r="AC23">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD23">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE23">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF23">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="24" spans="1:31" ht="144" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32" ht="144" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>38</v>
       </c>
@@ -14434,12 +15844,24 @@
       <c r="AB24" s="2" t="s">
         <v>978</v>
       </c>
+      <c r="AC24">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD24">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE24">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF24">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="25" spans="1:31" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>38</v>
       </c>
@@ -14522,12 +15944,24 @@
       <c r="AB25" s="2" t="s">
         <v>978</v>
       </c>
+      <c r="AC25">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD25">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE25">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF25">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="26" spans="1:31" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -14602,12 +16036,24 @@
       <c r="AB26" s="2" t="s">
         <v>981</v>
       </c>
+      <c r="AC26">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD26">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE26">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF26">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="27" spans="1:31" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:32" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>38</v>
       </c>
@@ -14682,12 +16128,24 @@
       <c r="AB27" s="2" t="s">
         <v>983</v>
       </c>
+      <c r="AC27">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD27">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE27">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF27">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="28" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
@@ -14762,12 +16220,24 @@
       <c r="AB28" s="2" t="s">
         <v>981</v>
       </c>
+      <c r="AC28">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD28">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE28">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF28">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="29" spans="1:31" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:32" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>38</v>
       </c>
@@ -14842,12 +16312,24 @@
       <c r="AB29" s="2" t="s">
         <v>949</v>
       </c>
+      <c r="AC29">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD29">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE29">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF29">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="30" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
@@ -14924,12 +16406,24 @@
       <c r="AB30" s="2" t="s">
         <v>988</v>
       </c>
+      <c r="AC30">
+        <f>Notes!$C$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>912.5</v>
+      </c>
+      <c r="AD30">
+        <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>1825</v>
+      </c>
       <c r="AE30">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2522880000</v>
+      </c>
+      <c r="AF30">
+        <f>Notes!$F$7 * Notes!$D$10 * Notes!$C$13</f>
+        <v>2737.5</v>
       </c>
     </row>
-    <row r="31" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
@@ -15002,12 +16496,24 @@
       <c r="AB31" s="2" t="s">
         <v>993</v>
       </c>
+      <c r="AC31">
+        <f>Notes!$C$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>7300</v>
+      </c>
+      <c r="AD31">
+        <f>Notes!$D$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>14600</v>
+      </c>
       <c r="AE31">
-        <f>Notes!$E$7 * 8 * Notes!$E$10 * Notes!$C$13</f>
-        <v>80732160000</v>
+        <f>Notes!$E$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>20183040000</v>
+      </c>
+      <c r="AF31">
+        <f>Notes!$F$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>21900</v>
       </c>
     </row>
-    <row r="32" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
@@ -15090,12 +16596,24 @@
       <c r="AB32" s="2" t="s">
         <v>995</v>
       </c>
+      <c r="AC32">
+        <f>Notes!$C$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>7300</v>
+      </c>
+      <c r="AD32">
+        <f>Notes!$D$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>14600</v>
+      </c>
       <c r="AE32">
-        <f>Notes!$E$7 * 8 * Notes!$E$10 * Notes!$C$13</f>
-        <v>80732160000</v>
+        <f>Notes!$E$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>20183040000</v>
+      </c>
+      <c r="AF32">
+        <f>Notes!$F$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>21900</v>
       </c>
     </row>
-    <row r="33" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>38</v>
       </c>
@@ -15176,12 +16694,24 @@
       <c r="AB33" s="2" t="s">
         <v>993</v>
       </c>
+      <c r="AC33">
+        <f>Notes!$C$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>7300</v>
+      </c>
+      <c r="AD33">
+        <f>Notes!$D$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>14600</v>
+      </c>
       <c r="AE33">
-        <f>Notes!$E$7 * 8 * Notes!$E$10 * Notes!$C$13</f>
-        <v>80732160000</v>
+        <f>Notes!$E$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>20183040000</v>
+      </c>
+      <c r="AF33">
+        <f>Notes!$F$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>21900</v>
       </c>
     </row>
-    <row r="34" spans="1:31" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -15256,12 +16786,24 @@
       <c r="AB34" s="2" t="s">
         <v>995</v>
       </c>
+      <c r="AC34">
+        <f>Notes!$C$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>7300</v>
+      </c>
+      <c r="AD34">
+        <f>Notes!$D$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>14600</v>
+      </c>
       <c r="AE34">
-        <f>Notes!$E$7 * 8 * Notes!$E$10 * Notes!$C$13</f>
-        <v>80732160000</v>
+        <f>Notes!$E$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>20183040000</v>
+      </c>
+      <c r="AF34">
+        <f>Notes!$F$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>21900</v>
       </c>
     </row>
-    <row r="35" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>38</v>
       </c>
@@ -15334,12 +16876,24 @@
       <c r="AB35" s="2" t="s">
         <v>993</v>
       </c>
+      <c r="AC35">
+        <f>Notes!$C$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>7300</v>
+      </c>
+      <c r="AD35">
+        <f>Notes!$D$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>14600</v>
+      </c>
       <c r="AE35">
-        <f>Notes!$E$7 * 8 * Notes!$E$10 * Notes!$C$13</f>
-        <v>80732160000</v>
+        <f>Notes!$E$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>20183040000</v>
+      </c>
+      <c r="AF35">
+        <f>Notes!$F$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>21900</v>
       </c>
     </row>
-    <row r="36" spans="1:31" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
@@ -15412,12 +16966,24 @@
       <c r="AB36" s="2" t="s">
         <v>993</v>
       </c>
+      <c r="AC36">
+        <f>Notes!$C$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>7300</v>
+      </c>
+      <c r="AD36">
+        <f>Notes!$D$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>14600</v>
+      </c>
       <c r="AE36">
-        <f>Notes!$E$7 * 8 * Notes!$E$10 * Notes!$C$13</f>
-        <v>80732160000</v>
+        <f>Notes!$E$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>20183040000</v>
+      </c>
+      <c r="AF36">
+        <f>Notes!$F$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>21900</v>
       </c>
     </row>
-    <row r="37" spans="1:31" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:32" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>826</v>
       </c>
@@ -15490,9 +17056,21 @@
       <c r="AB37" s="2" t="s">
         <v>1005</v>
       </c>
+      <c r="AC37">
+        <f>Notes!$C$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>7300</v>
+      </c>
+      <c r="AD37">
+        <f>Notes!$D$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>14600</v>
+      </c>
       <c r="AE37">
-        <f>Notes!$E$7 * 8 * Notes!$E$10 * Notes!$C$13</f>
-        <v>80732160000</v>
+        <f>Notes!$E$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>20183040000</v>
+      </c>
+      <c r="AF37">
+        <f>Notes!$F$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
+        <v>21900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixed in 6hrPlevPt zg
</commit_message>
<xml_diff>
--- a/eerie_first_draft/PRIMAVERA_top_50.xlsx
+++ b/eerie_first_draft/PRIMAVERA_top_50.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\eerie\dreq\eerie_dreq\eerie_first_draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE2FF739-95CF-47AD-9443-E75C24E7539B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CABCC50-DE93-4CF2-B344-FE1A061C451C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -4223,8 +4223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4465,23 +4465,23 @@
       </c>
       <c r="C17" s="6">
         <f>SUM('6hrPlevPt'!$AC$2:$AC$100) / POWER(1024,3)</f>
-        <v>1.6996636986732483E-5</v>
+        <v>3.7392601370811462E-5</v>
       </c>
       <c r="D17" s="6">
         <f>SUM('6hrPlevPt'!$AD$2:$AD$100) / POWER(1024,3)</f>
-        <v>3.3993273973464966E-5</v>
+        <v>7.4785202741622925E-5</v>
       </c>
       <c r="E17" s="6">
         <f>SUM('6hrPlevPt'!$AE$2:$AE$100) / POWER(1024,3)</f>
-        <v>46.992301940917969</v>
+        <v>103.38306427001953</v>
       </c>
       <c r="F17" s="6">
         <f>SUM('6hrPlevPt'!$AF$2:$AF$100) / POWER(1024,3)</f>
-        <v>5.0989910960197449E-5</v>
+        <v>1.1217780411243439E-4</v>
       </c>
       <c r="G17" s="6">
         <f>SUM(C17:F17)</f>
-        <v>46.992403920739889</v>
+        <v>103.38328862562776</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
@@ -4657,23 +4657,23 @@
       </c>
       <c r="C29" s="6">
         <f>SUM(C17:C28)</f>
-        <v>1.2230128049850464E-4</v>
+        <v>1.4269724488258362E-4</v>
       </c>
       <c r="D29" s="6">
         <f t="shared" ref="D29:G29" si="1">SUM(D17:D28)</f>
-        <v>2.4460256099700928E-4</v>
+        <v>2.8539448976516724E-4</v>
       </c>
       <c r="E29" s="6">
         <f t="shared" si="1"/>
-        <v>414.40446549095213</v>
+        <v>470.7952278200537</v>
       </c>
       <c r="F29" s="6">
         <f t="shared" si="1"/>
-        <v>3.6690384149551392E-4</v>
+        <v>4.2809173464775085E-4</v>
       </c>
       <c r="G29" s="6">
         <f t="shared" si="1"/>
-        <v>414.40519929863513</v>
+        <v>470.79608400352299</v>
       </c>
     </row>
   </sheetData>
@@ -4695,7 +4695,7 @@
   <dimension ref="A1:AF6"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AE2" sqref="AE2"/>
+      <selection activeCell="AF3" sqref="AF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4963,20 +4963,20 @@
         <v>247</v>
       </c>
       <c r="AC3">
-        <f>Notes!$C$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>3650</v>
+        <f>Notes!$C$7 * 7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>25550</v>
       </c>
       <c r="AD3">
-        <f>Notes!$D$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>7300</v>
+        <f>Notes!$D$7 * 7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>51100</v>
       </c>
       <c r="AE3">
-        <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10091520000</v>
+        <f>Notes!$E$7 * 7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>70640640000</v>
       </c>
       <c r="AF3">
-        <f>Notes!$F$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>10950</v>
+        <f>Notes!$F$7 * 7 * Notes!$E$10 * Notes!$C$13</f>
+        <v>76650</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -12768,8 +12768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2:AF2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13644,7 +13644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView topLeftCell="I31" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="AC37" sqref="AC37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Bug fix for alevel variables in Amon
</commit_message>
<xml_diff>
--- a/eerie_first_draft/PRIMAVERA_top_50.xlsx
+++ b/eerie_first_draft/PRIMAVERA_top_50.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\eerie\dreq\eerie_dreq\eerie_first_draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF2368D-86D1-4927-854B-C39EEDB43C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C3742E-1FCA-4624-8BC7-4D582A133F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -5762,7 +5762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -6057,11 +6057,11 @@
       </c>
       <c r="C19" s="4">
         <f>SUM(Amon!$AC$2:$AC$100) / POWER(1024,3)</f>
-        <v>156.54959678649902</v>
+        <v>63.615560531616211</v>
       </c>
       <c r="D19" s="4">
         <f>SUM(Amon!$AD$2:$AD$100) / POWER(1024,3)</f>
-        <v>4.7441571950912476E-5</v>
+        <v>1.9278377294540405E-5</v>
       </c>
       <c r="E19" s="4">
         <f>SUM(Amon!$AE$2:$AE$100) / POWER(1024,3)</f>
@@ -6069,11 +6069,11 @@
       </c>
       <c r="F19" s="4">
         <f>SUM(Amon!$AF$2:$AF$100) / POWER(1024,3)</f>
-        <v>124.365234375</v>
+        <v>128.759765625</v>
       </c>
       <c r="G19" s="7">
         <f t="shared" si="0"/>
-        <v>346.49810766801238</v>
+        <v>257.95857449993491</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
@@ -6207,11 +6207,11 @@
       </c>
       <c r="C25" s="7">
         <f>SUM(C17:C24)</f>
-        <v>1054.9395216489211</v>
+        <v>962.00548539403826</v>
       </c>
       <c r="D25" s="7">
         <f>SUM(D17:D24)</f>
-        <v>2.8826761990785599E-4</v>
+        <v>2.6010442525148392E-4</v>
       </c>
       <c r="E25" s="7">
         <f>SUM(E17:E24)</f>
@@ -6219,11 +6219,11 @@
       </c>
       <c r="F25" s="7">
         <f>SUM(F17:F24)</f>
-        <v>839.55759814707562</v>
+        <v>843.95212939707562</v>
       </c>
       <c r="G25" s="7">
         <f>SUM(G17:G24)</f>
-        <v>2602.3463286343031</v>
+        <v>2513.8067954662256</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
@@ -11384,8 +11384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AF76"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AE57" sqref="AE57"/>
+    <sheetView tabSelected="1" topLeftCell="G71" workbookViewId="0">
+      <selection activeCell="AF76" sqref="AF76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15934,20 +15934,20 @@
         <v>620</v>
       </c>
       <c r="AC46">
-        <f>Notes!$C$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>16829184000</v>
+        <f>Notes!$C$7 * Notes!$K$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>197990400</v>
       </c>
       <c r="AD46">
-        <f>Notes!$D$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>5100</v>
+        <f>Notes!$D$7 * Notes!$L$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
       </c>
       <c r="AE46">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>7050240000</v>
       </c>
       <c r="AF46">
-        <f>Notes!$F$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>13369344000</v>
+        <f>Notes!$F$7 * Notes!$N$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>14155776000</v>
       </c>
     </row>
     <row r="47" spans="1:32" ht="100.8" x14ac:dyDescent="0.3">
@@ -16026,20 +16026,20 @@
         <v>630</v>
       </c>
       <c r="AC47">
-        <f>Notes!$C$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>16829184000</v>
+        <f>Notes!$C$7 * Notes!$K$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>197990400</v>
       </c>
       <c r="AD47">
-        <f>Notes!$D$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>5100</v>
+        <f>Notes!$D$7 * Notes!$L$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
       </c>
       <c r="AE47">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>7050240000</v>
       </c>
       <c r="AF47">
-        <f>Notes!$F$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>13369344000</v>
+        <f>Notes!$F$7 * Notes!$N$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>14155776000</v>
       </c>
     </row>
     <row r="48" spans="1:32" ht="100.8" x14ac:dyDescent="0.3">
@@ -16118,20 +16118,20 @@
         <v>639</v>
       </c>
       <c r="AC48">
-        <f>Notes!$C$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>16829184000</v>
+        <f>Notes!$C$7 * Notes!$K$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>197990400</v>
       </c>
       <c r="AD48">
-        <f>Notes!$D$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>5100</v>
+        <f>Notes!$D$7 * Notes!$L$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
       </c>
       <c r="AE48">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>7050240000</v>
       </c>
       <c r="AF48">
-        <f>Notes!$F$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>13369344000</v>
+        <f>Notes!$F$7 * Notes!$N$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>14155776000</v>
       </c>
     </row>
     <row r="49" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
@@ -16210,20 +16210,20 @@
         <v>639</v>
       </c>
       <c r="AC49">
-        <f>Notes!$C$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>16829184000</v>
+        <f>Notes!$C$7 * Notes!$K$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>197990400</v>
       </c>
       <c r="AD49">
-        <f>Notes!$D$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>5100</v>
+        <f>Notes!$D$7 * Notes!$L$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
       </c>
       <c r="AE49">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>7050240000</v>
       </c>
       <c r="AF49">
-        <f>Notes!$F$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>13369344000</v>
+        <f>Notes!$F$7 * Notes!$N$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>14155776000</v>
       </c>
     </row>
     <row r="50" spans="1:32" ht="57.6" x14ac:dyDescent="0.3">
@@ -18584,20 +18584,20 @@
         <v>639</v>
       </c>
       <c r="AC75">
-        <f>Notes!$C$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>16829184000</v>
+        <f>Notes!$C$7 * Notes!$K$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>197990400</v>
       </c>
       <c r="AD75">
-        <f>Notes!$D$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>5100</v>
+        <f>Notes!$D$7 * Notes!$L$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
       </c>
       <c r="AE75">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>7050240000</v>
       </c>
       <c r="AF75">
-        <f>Notes!$F$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>13369344000</v>
+        <f>Notes!$F$7 * Notes!$N$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>14155776000</v>
       </c>
     </row>
     <row r="76" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
@@ -18674,20 +18674,20 @@
         <v>639</v>
       </c>
       <c r="AC76">
-        <f>Notes!$C$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>16829184000</v>
+        <f>Notes!$C$7 * Notes!$K$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>197990400</v>
       </c>
       <c r="AD76">
-        <f>Notes!$D$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>5100</v>
+        <f>Notes!$D$7 * Notes!$L$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>60</v>
       </c>
       <c r="AE76">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
         <v>7050240000</v>
       </c>
       <c r="AF76">
-        <f>Notes!$F$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>13369344000</v>
+        <f>Notes!$F$7 * Notes!$N$7 * Notes!$C$10 * Notes!$C$13</f>
+        <v>14155776000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Includes BSC. AWI levels assumed at 137.
</commit_message>
<xml_diff>
--- a/eerie_first_draft/PRIMAVERA_top_50.xlsx
+++ b/eerie_first_draft/PRIMAVERA_top_50.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\eerie\dreq\eerie_dreq\eerie_first_draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C3742E-1FCA-4624-8BC7-4D582A133F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7A0CEE-AE28-4BB7-8292-E8E9B4C6E3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -45,10 +45,37 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={DFAB5DB5-5817-44C8-BB8D-A15ACCFE5CB8}</author>
+    <author>tc={D1AFC42F-2ADB-44C1-BC7D-BA47F266CDC1}</author>
+  </authors>
+  <commentList>
+    <comment ref="K7" authorId="0" shapeId="0" xr:uid="{DFAB5DB5-5817-44C8-BB8D-A15ACCFE5CB8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I have assumed 137 atmosphere levels for AWI</t>
+      </text>
+    </comment>
+    <comment ref="L7" authorId="1" shapeId="0" xr:uid="{D1AFC42F-2ADB-44C1-BC7D-BA47F266CDC1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I have assumed 137 atmosphere levels for BSC</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -61,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +101,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -87,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -100,7 +127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000005000000}">
       <text>
         <r>
           <rPr>
@@ -113,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000006000000}">
       <text>
         <r>
           <rPr>
@@ -126,7 +153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000007000000}">
       <text>
         <r>
           <rPr>
@@ -139,7 +166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000008000000}">
       <text>
         <r>
           <rPr>
@@ -156,7 +183,7 @@
 </comments>
 </file>
 
-<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -276,6 +303,120 @@
     <author/>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Default priority (generally overridden by settings in "requestVar" record)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>NetCDF Global Attribute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name of variable in file</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CMOR directive</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CMOR name, unique within table</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CMOR variable identifier</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MIP variable identifier</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Structure identifier</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{CFE42800-36EE-4772-80B2-4F55C218D7A8}">
       <text>
         <r>
@@ -384,7 +525,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -498,7 +639,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -612,7 +753,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -726,7 +867,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -840,7 +981,7 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -954,7 +1095,7 @@
 </comments>
 </file>
 
-<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -1068,120 +1209,6 @@
 </comments>
 </file>
 
-<file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Default priority (generally overridden by settings in "requestVar" record)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000002000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>NetCDF Global Attribute</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000003000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Name of variable in file</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CMOR directive</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CMOR name, unique within table</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CMOR variable identifier</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>MIP variable identifier</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1400-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Structure identifier</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4237" uniqueCount="1385">
   <si>
@@ -5347,7 +5374,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5376,6 +5403,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -5414,14 +5453,14 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5437,6 +5476,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Seddon, Jon" id="{160E1B36-7B5A-443B-9D8B-DD525A48728B}" userId="S::jon.seddon@metoffice.gov.uk::a2ecb1af-462c-47a7-a0d0-b1beb0b91723" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5758,12 +5803,23 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="K7" dT="2023-01-31T15:49:33.70" personId="{160E1B36-7B5A-443B-9D8B-DD525A48728B}" id="{DFAB5DB5-5817-44C8-BB8D-A15ACCFE5CB8}">
+    <text>I have assumed 137 atmosphere levels for AWI</text>
+  </threadedComment>
+  <threadedComment ref="L7" dT="2023-01-31T16:39:21.14" personId="{160E1B36-7B5A-443B-9D8B-DD525A48728B}" id="{D1AFC42F-2ADB-44C1-BC7D-BA47F266CDC1}">
+    <text>I have assumed 137 atmosphere levels for BSC</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5772,7 +5828,8 @@
     <col min="2" max="2" width="60.6640625" customWidth="1"/>
     <col min="3" max="4" width="8.88671875" customWidth="1"/>
     <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="10" max="18" width="9" bestFit="1" customWidth="1"/>
   </cols>
@@ -5805,30 +5862,30 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>1006</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6" t="s">
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
         <v>1011</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6" t="s">
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7" t="s">
         <v>1019</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6" t="s">
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7" t="s">
         <v>1020</v>
       </c>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
@@ -5881,63 +5938,64 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <v>6599680</v>
       </c>
-      <c r="D7" s="8">
-        <v>2</v>
-      </c>
-      <c r="E7" s="8">
+      <c r="D7" s="6">
+        <v>2140702</v>
+      </c>
+      <c r="E7" s="6">
         <f>1440*1920</f>
         <v>2764800</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <v>5242880</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="6">
         <v>7402886</v>
       </c>
-      <c r="H7" s="8">
-        <v>2</v>
-      </c>
-      <c r="I7" s="8">
+      <c r="H7" s="6">
+        <f>4322 * 3059</f>
+        <v>13220998</v>
+      </c>
+      <c r="I7" s="6">
         <f>4322 * 3606</f>
         <v>15585132</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="6">
         <v>3729001</v>
       </c>
-      <c r="K7" s="8">
-        <v>1</v>
-      </c>
-      <c r="L7" s="8">
-        <v>1</v>
-      </c>
-      <c r="M7" s="8">
+      <c r="K7" s="6">
+        <v>137</v>
+      </c>
+      <c r="L7" s="6">
+        <v>137</v>
+      </c>
+      <c r="M7" s="6">
         <v>85</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="6">
         <v>90</v>
       </c>
-      <c r="O7" s="8">
+      <c r="O7" s="6">
         <v>69</v>
       </c>
-      <c r="P7" s="8">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="8">
+      <c r="P7" s="6">
         <v>75</v>
       </c>
-      <c r="R7" s="8">
+      <c r="Q7" s="6">
+        <v>75</v>
+      </c>
+      <c r="R7" s="6">
         <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>1013</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
@@ -5973,13 +6031,13 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="8" t="s">
         <v>1023</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
@@ -6011,7 +6069,7 @@
       </c>
       <c r="D17" s="4">
         <f>SUM('6hrPlevPt'!$AD$2:$AD$100) / POWER(1024,3)</f>
-        <v>7.4785202741622925E-5</v>
+        <v>80.046416539698839</v>
       </c>
       <c r="E17" s="4">
         <f>SUM('6hrPlevPt'!$AE$2:$AE$100) / POWER(1024,3)</f>
@@ -6021,9 +6079,9 @@
         <f>SUM('6hrPlevPt'!$AF$2:$AF$100) / POWER(1024,3)</f>
         <v>196.044921875</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="5">
         <f>SUM(C17:F17)</f>
-        <v>546.20726434513927</v>
+        <v>626.25360609963536</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
@@ -6036,7 +6094,7 @@
       </c>
       <c r="D18" s="4">
         <f>SUM(Prim6hr!$AD$2:$AD$100) / POWER(1024,3)</f>
-        <v>6.7986547946929932E-6</v>
+        <v>7.2769469581544399</v>
       </c>
       <c r="E18" s="4">
         <f>SUM(Prim6hr!$AE$2:$AE$100) / POWER(1024,3)</f>
@@ -6046,9 +6104,9 @@
         <f>SUM(Prim6hr!$AF$2:$AF$100) / POWER(1024,3)</f>
         <v>17.822265625</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="5">
         <f t="shared" ref="G18:G24" si="0">SUM(C18:F18)</f>
-        <v>49.655205849558115</v>
+        <v>56.93214600905776</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
@@ -6057,11 +6115,11 @@
       </c>
       <c r="C19" s="4">
         <f>SUM(Amon!$AC$2:$AC$100) / POWER(1024,3)</f>
-        <v>63.615560531616211</v>
+        <v>214.08019065856934</v>
       </c>
       <c r="D19" s="4">
         <f>SUM(Amon!$AD$2:$AD$100) / POWER(1024,3)</f>
-        <v>1.9278377294540405E-5</v>
+        <v>69.440017137676477</v>
       </c>
       <c r="E19" s="4">
         <f>SUM(Amon!$AE$2:$AE$100) / POWER(1024,3)</f>
@@ -6071,9 +6129,9 @@
         <f>SUM(Amon!$AF$2:$AF$100) / POWER(1024,3)</f>
         <v>128.759765625</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="5">
         <f t="shared" si="0"/>
-        <v>257.95857449993491</v>
+        <v>477.86320248618722</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
@@ -6086,7 +6144,7 @@
       </c>
       <c r="D20" s="4">
         <f>SUM(Oday!$AD$2:$AD$100) / POWER(1024,3)</f>
-        <v>5.0989910960197449E-6</v>
+        <v>33.706875541247427</v>
       </c>
       <c r="E20" s="4">
         <f>SUM(Oday!$AE$2:$AE$100) / POWER(1024,3)</f>
@@ -6096,9 +6154,9 @@
         <f>SUM(Oday!$AF$2:$AF$100) / POWER(1024,3)</f>
         <v>9.5070714480243623</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="5">
         <f t="shared" si="0"/>
-        <v>68.11492609558627</v>
+        <v>101.8217965378426</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
@@ -6111,7 +6169,7 @@
       </c>
       <c r="D21" s="4">
         <f>SUM(Omon!$AD$2:$AD$101) / POWER(1024,3)</f>
-        <v>8.3819031715393066E-7</v>
+        <v>196.88509220257401</v>
       </c>
       <c r="E21" s="4">
         <f>SUM(Omon!$AE$2:$AE$101) / POWER(1024,3)</f>
@@ -6121,9 +6179,9 @@
         <f>SUM(Omon!$AF$2:$AF$101) / POWER(1024,3)</f>
         <v>94.185124263167381</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="5">
         <f t="shared" ref="G21" si="1">SUM(C21:F21)</f>
-        <v>427.83215593546629</v>
+        <v>624.71724729984999</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.3">
@@ -6136,7 +6194,7 @@
       </c>
       <c r="D22" s="4">
         <f>SUM(SIday!$AD$2:$AD$101) / POWER(1024,3)</f>
-        <v>8.4983184933662415E-6</v>
+        <v>46.761737461201847</v>
       </c>
       <c r="E22" s="4">
         <f>SUM(SIday!$AE$2:$AE$101) / POWER(1024,3)</f>
@@ -6146,9 +6204,9 @@
         <f>SUM(SIday!$AF$2:$AF$101) / POWER(1024,3)</f>
         <v>18.284713523462415</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="5">
         <f t="shared" si="0"/>
-        <v>104.38675477635115</v>
+        <v>151.14848373923451</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.3">
@@ -6161,7 +6219,7 @@
       </c>
       <c r="D23" s="4">
         <f>SUM(SImon!$AD$2:$AD$101) / POWER(1024,3)</f>
-        <v>3.3527612686157227E-7</v>
+        <v>2.2163425013422966</v>
       </c>
       <c r="E23" s="4">
         <f>SUM(SImon!$AE$2:$AE$101) / POWER(1024,3)</f>
@@ -6171,9 +6229,9 @@
         <f>SUM(SImon!$AF$2:$AF$101) / POWER(1024,3)</f>
         <v>0.62512250617146492</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="5">
         <f t="shared" ref="G23" si="2">SUM(C23:F23)</f>
-        <v>4.4787896610796452</v>
+        <v>6.6951318271458149</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
@@ -6186,7 +6244,7 @@
       </c>
       <c r="D24" s="4">
         <f>SUM(day!$AD$2:$AD$100) / POWER(1024,3)</f>
-        <v>1.444714143872261E-4</v>
+        <v>154.63512286078185</v>
       </c>
       <c r="E24" s="4">
         <f>SUM(day!$AE$2:$AE$100) / POWER(1024,3)</f>
@@ -6196,34 +6254,34 @@
         <f>SUM(day!$AF$2:$AF$100) / POWER(1024,3)</f>
         <v>378.72314453125</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="5">
         <f t="shared" si="0"/>
-        <v>1055.1731243031099</v>
+        <v>1209.8081026924774</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>1024</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="5">
         <f>SUM(C17:C24)</f>
-        <v>962.00548539403826</v>
-      </c>
-      <c r="D25" s="7">
+        <v>1112.4701155209914</v>
+      </c>
+      <c r="D25" s="5">
         <f>SUM(D17:D24)</f>
-        <v>2.6010442525148392E-4</v>
-      </c>
-      <c r="E25" s="7">
+        <v>590.96855120267719</v>
+      </c>
+      <c r="E25" s="5">
         <f>SUM(E17:E24)</f>
         <v>707.84892057068646</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="5">
         <f>SUM(F17:F24)</f>
         <v>843.95212939707562</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="5">
         <f>SUM(G17:G24)</f>
-        <v>2513.8067954662256</v>
+        <v>3255.2397166914307</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.3">
@@ -6245,7 +6303,7 @@
       </c>
       <c r="D28" s="4">
         <f>SUM(Ofx!$AD$2:$AD$101) / POWER(1024,3)</f>
-        <v>4.1909515857696533E-8</v>
+        <v>7.1107655251398683</v>
       </c>
       <c r="E28" s="4">
         <f>SUM(Ofx!$AE$2:$AE$101) / POWER(1024,3)</f>
@@ -6255,9 +6313,9 @@
         <f>SUM(Ofx!$AF$2:$AF$101) / POWER(1024,3)</f>
         <v>3.3860802417621017</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="5">
         <f t="shared" ref="G28" si="3">SUM(C28:F28)</f>
-        <v>15.439676628448069</v>
+        <v>22.550442111678421</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.3">
@@ -6266,11 +6324,11 @@
       </c>
       <c r="C29" s="4">
         <f>SUM(fx!$AC$2:$AC$101) / POWER(1024,3)</f>
-        <v>0.12292861938476563</v>
+        <v>2.2127151489257813</v>
       </c>
       <c r="D29" s="4">
         <f>SUM(fx!$AD$2:$AD$101) / POWER(1024,3)</f>
-        <v>3.7252902984619141E-8</v>
+        <v>0.71772627532482147</v>
       </c>
       <c r="E29" s="4">
         <f>SUM(fx!$AE$2:$AE$101) / POWER(1024,3)</f>
@@ -6280,34 +6338,34 @@
         <f>SUM(fx!$AF$2:$AF$101) / POWER(1024,3)</f>
         <v>1.18408203125</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="5">
         <f t="shared" ref="G29" si="4">SUM(C29:F29)</f>
-        <v>1.8992424383759499</v>
+        <v>4.706755205988884</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="3" t="s">
         <v>1382</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="5">
         <f>SUM(C28:C29)</f>
-        <v>3.7942364765331149</v>
-      </c>
-      <c r="D30" s="7">
+        <v>5.8840230060741305</v>
+      </c>
+      <c r="D30" s="5">
         <f t="shared" ref="D30:G30" si="5">SUM(D28:D29)</f>
-        <v>7.9162418842315674E-8</v>
-      </c>
-      <c r="E30" s="7">
+        <v>7.8284918004646897</v>
+      </c>
+      <c r="E30" s="5">
         <f t="shared" si="5"/>
         <v>8.9745202381163836</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="5">
         <f t="shared" si="5"/>
         <v>4.5701622730121017</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="5">
         <f t="shared" si="5"/>
-        <v>17.338919066824019</v>
+        <v>27.257197317667305</v>
       </c>
     </row>
   </sheetData>
@@ -6321,6 +6379,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6516,7 +6575,7 @@
       </c>
       <c r="AD2">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE2">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -6606,7 +6665,7 @@
       </c>
       <c r="AD3">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE3">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -6696,7 +6755,7 @@
       </c>
       <c r="AD4">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE4">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -6786,7 +6845,7 @@
       </c>
       <c r="AD5">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE5">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -6878,7 +6937,7 @@
       </c>
       <c r="AD6">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE6">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -6968,7 +7027,7 @@
       </c>
       <c r="AD7">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE7">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -7058,7 +7117,7 @@
       </c>
       <c r="AD8">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE8">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -7148,7 +7207,7 @@
       </c>
       <c r="AD9">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE9">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -7240,7 +7299,7 @@
       </c>
       <c r="AD10">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE10">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -7332,7 +7391,7 @@
       </c>
       <c r="AD11">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE11">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -7424,7 +7483,7 @@
       </c>
       <c r="AD12">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE12">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -7516,7 +7575,7 @@
       </c>
       <c r="AD13">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE13">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -7606,7 +7665,7 @@
       </c>
       <c r="AD14">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE14">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -7706,7 +7765,7 @@
       </c>
       <c r="AD15">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE15">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -7796,7 +7855,7 @@
       </c>
       <c r="AD16">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE16">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -7888,7 +7947,7 @@
       </c>
       <c r="AD17">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE17">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -7980,7 +8039,7 @@
       </c>
       <c r="AD18">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE18">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -8072,7 +8131,7 @@
       </c>
       <c r="AD19">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE19">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -8164,7 +8223,7 @@
       </c>
       <c r="AD20">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE20">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -8254,7 +8313,7 @@
       </c>
       <c r="AD21">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE21">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -8344,7 +8403,7 @@
       </c>
       <c r="AD22">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE22">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -8434,7 +8493,7 @@
       </c>
       <c r="AD23">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE23">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -8534,7 +8593,7 @@
       </c>
       <c r="AD24">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE24">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -8634,7 +8693,7 @@
       </c>
       <c r="AD25">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE25">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -8726,7 +8785,7 @@
       </c>
       <c r="AD26">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE26">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -8818,7 +8877,7 @@
       </c>
       <c r="AD27">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE27">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -8910,7 +8969,7 @@
       </c>
       <c r="AD28">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE28">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -9002,7 +9061,7 @@
       </c>
       <c r="AD29">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE29">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -9096,7 +9155,7 @@
       </c>
       <c r="AD30">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE30">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -9186,7 +9245,7 @@
       </c>
       <c r="AD31">
         <f>Notes!$D$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
-        <v>14600</v>
+        <v>15627124600</v>
       </c>
       <c r="AE31">
         <f>Notes!$E$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
@@ -9286,7 +9345,7 @@
       </c>
       <c r="AD32">
         <f>Notes!$D$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
-        <v>14600</v>
+        <v>15627124600</v>
       </c>
       <c r="AE32">
         <f>Notes!$E$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
@@ -9384,7 +9443,7 @@
       </c>
       <c r="AD33">
         <f>Notes!$D$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
-        <v>14600</v>
+        <v>15627124600</v>
       </c>
       <c r="AE33">
         <f>Notes!$E$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
@@ -9476,7 +9535,7 @@
       </c>
       <c r="AD34">
         <f>Notes!$D$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
-        <v>14600</v>
+        <v>15627124600</v>
       </c>
       <c r="AE34">
         <f>Notes!$E$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
@@ -9566,7 +9625,7 @@
       </c>
       <c r="AD35">
         <f>Notes!$D$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
-        <v>14600</v>
+        <v>15627124600</v>
       </c>
       <c r="AE35">
         <f>Notes!$E$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
@@ -9656,7 +9715,7 @@
       </c>
       <c r="AD36">
         <f>Notes!$D$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
-        <v>14600</v>
+        <v>15627124600</v>
       </c>
       <c r="AE36">
         <f>Notes!$E$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
@@ -9746,7 +9805,7 @@
       </c>
       <c r="AD37">
         <f>Notes!$D$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
-        <v>14600</v>
+        <v>15627124600</v>
       </c>
       <c r="AE37">
         <f>Notes!$E$7 * 8 * Notes!$D$10 * Notes!$C$13</f>
@@ -9961,7 +10020,7 @@
       </c>
       <c r="AD2">
         <f>Notes!$D$7 * Notes!$C$13</f>
-        <v>5</v>
+        <v>5351755</v>
       </c>
       <c r="AE2">
         <f>Notes!$E$7 *  Notes!$C$13</f>
@@ -10049,7 +10108,7 @@
       </c>
       <c r="AD3">
         <f>Notes!$D$7 * Notes!$C$13</f>
-        <v>5</v>
+        <v>5351755</v>
       </c>
       <c r="AE3">
         <f>Notes!$E$7 *  Notes!$C$13</f>
@@ -10143,7 +10202,7 @@
       </c>
       <c r="AD4">
         <f>Notes!$D$7 * Notes!$C$13</f>
-        <v>5</v>
+        <v>5351755</v>
       </c>
       <c r="AE4">
         <f>Notes!$E$7 *  Notes!$C$13</f>
@@ -10235,7 +10294,7 @@
       </c>
       <c r="AD5">
         <f>Notes!$D$7 * Notes!$C$13</f>
-        <v>5</v>
+        <v>5351755</v>
       </c>
       <c r="AE5">
         <f>Notes!$E$7 *  Notes!$C$13</f>
@@ -10329,7 +10388,7 @@
       </c>
       <c r="AD6">
         <f>Notes!$D$7 * Notes!$C$13</f>
-        <v>5</v>
+        <v>5351755</v>
       </c>
       <c r="AE6">
         <f>Notes!$E$7 *  Notes!$C$13</f>
@@ -10419,7 +10478,7 @@
       </c>
       <c r="AD7">
         <f>Notes!$D$7 * Notes!$C$13</f>
-        <v>5</v>
+        <v>5351755</v>
       </c>
       <c r="AE7">
         <f>Notes!$E$7 *  Notes!$C$13</f>
@@ -10513,7 +10572,7 @@
       </c>
       <c r="AD8">
         <f>Notes!$D$7 * Notes!$C$13</f>
-        <v>5</v>
+        <v>5351755</v>
       </c>
       <c r="AE8">
         <f>Notes!$E$7 *  Notes!$C$13</f>
@@ -10601,11 +10660,11 @@
       </c>
       <c r="AC9">
         <f>Notes!$C$7 * Notes!$K$7 * Notes!$C$13</f>
-        <v>16499200</v>
+        <v>2260390400</v>
       </c>
       <c r="AD9">
         <f>Notes!$D$7 * Notes!$L$7 * Notes!$C$13</f>
-        <v>5</v>
+        <v>733190435</v>
       </c>
       <c r="AE9">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$13</f>
@@ -10812,7 +10871,7 @@
       </c>
       <c r="AD2">
         <f>Notes!$D$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>7300</v>
+        <v>7813562300</v>
       </c>
       <c r="AE2">
         <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
@@ -10900,7 +10959,7 @@
       </c>
       <c r="AD3">
         <f>Notes!$D$7 * 7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>51100</v>
+        <v>54694936100</v>
       </c>
       <c r="AE3">
         <f>Notes!$E$7 * 7 * Notes!$E$10 * Notes!$C$13</f>
@@ -10990,7 +11049,7 @@
       </c>
       <c r="AD4">
         <f>Notes!$D$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>7300</v>
+        <v>7813562300</v>
       </c>
       <c r="AE4">
         <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
@@ -11080,7 +11139,7 @@
       </c>
       <c r="AD5">
         <f>Notes!$D$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>7300</v>
+        <v>7813562300</v>
       </c>
       <c r="AE5">
         <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
@@ -11168,7 +11227,7 @@
       </c>
       <c r="AD6">
         <f>Notes!$D$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>7300</v>
+        <v>7813562300</v>
       </c>
       <c r="AE6">
         <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
@@ -11363,7 +11422,7 @@
       </c>
       <c r="AD2">
         <f>Notes!$D$7 * Notes!$E$10 * Notes!$C$13</f>
-        <v>7300</v>
+        <v>7813562300</v>
       </c>
       <c r="AE2">
         <f>Notes!$E$7 * Notes!$E$10 * Notes!$C$13</f>
@@ -11384,7 +11443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AF76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G71" workbookViewId="0">
+    <sheetView topLeftCell="G71" workbookViewId="0">
       <selection activeCell="AF76" sqref="AF76"/>
     </sheetView>
   </sheetViews>
@@ -11583,7 +11642,7 @@
       </c>
       <c r="AD2">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE2">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -11683,7 +11742,7 @@
       </c>
       <c r="AD3">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE3">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -11783,7 +11842,7 @@
       </c>
       <c r="AD4">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE4">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -11883,7 +11942,7 @@
       </c>
       <c r="AD5">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE5">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -11983,7 +12042,7 @@
       </c>
       <c r="AD6">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE6">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -12083,7 +12142,7 @@
       </c>
       <c r="AD7">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE7">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -12181,7 +12240,7 @@
       </c>
       <c r="AD8">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE8">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -12279,7 +12338,7 @@
       </c>
       <c r="AD9">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE9">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -12379,7 +12438,7 @@
       </c>
       <c r="AD10">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE10">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -12479,7 +12538,7 @@
       </c>
       <c r="AD11">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE11">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -12577,7 +12636,7 @@
       </c>
       <c r="AD12">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE12">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -12677,7 +12736,7 @@
       </c>
       <c r="AD13">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE13">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -12777,7 +12836,7 @@
       </c>
       <c r="AD14">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE14">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -12877,7 +12936,7 @@
       </c>
       <c r="AD15">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE15">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -12969,7 +13028,7 @@
       </c>
       <c r="AD16">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE16">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -13069,7 +13128,7 @@
       </c>
       <c r="AD17">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE17">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -13169,7 +13228,7 @@
       </c>
       <c r="AD18">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE18">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -13269,7 +13328,7 @@
       </c>
       <c r="AD19">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE19">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -13371,7 +13430,7 @@
       </c>
       <c r="AD20">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE20">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -13471,7 +13530,7 @@
       </c>
       <c r="AD21">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE21">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -13571,7 +13630,7 @@
       </c>
       <c r="AD22">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE22">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -13671,7 +13730,7 @@
       </c>
       <c r="AD23">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE23">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -13771,7 +13830,7 @@
       </c>
       <c r="AD24">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE24">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -13871,7 +13930,7 @@
       </c>
       <c r="AD25">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE25">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -13963,7 +14022,7 @@
       </c>
       <c r="AD26">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE26">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -14063,7 +14122,7 @@
       </c>
       <c r="AD27">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE27">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -14163,7 +14222,7 @@
       </c>
       <c r="AD28">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE28">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -14265,7 +14324,7 @@
       </c>
       <c r="AD29">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE29">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -14365,7 +14424,7 @@
       </c>
       <c r="AD30">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE30">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -14465,7 +14524,7 @@
       </c>
       <c r="AD31">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE31">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -14565,7 +14624,7 @@
       </c>
       <c r="AD32">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE32">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -14665,7 +14724,7 @@
       </c>
       <c r="AD33">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE33">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -14763,7 +14822,7 @@
       </c>
       <c r="AD34">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE34">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -14863,7 +14922,7 @@
       </c>
       <c r="AD35">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE35">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -14961,7 +15020,7 @@
       </c>
       <c r="AD36">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE36">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -15057,7 +15116,7 @@
       </c>
       <c r="AD37">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE37">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -15159,7 +15218,7 @@
       </c>
       <c r="AD38">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE38">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -15257,7 +15316,7 @@
       </c>
       <c r="AD39">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE39">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -15355,7 +15414,7 @@
       </c>
       <c r="AD40">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE40">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -15455,7 +15514,7 @@
       </c>
       <c r="AD41">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE41">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -15553,7 +15612,7 @@
       </c>
       <c r="AD42">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE42">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -15651,7 +15710,7 @@
       </c>
       <c r="AD43">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE43">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -15741,7 +15800,7 @@
       </c>
       <c r="AD44">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE44">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -15841,7 +15900,7 @@
       </c>
       <c r="AD45">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE45">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -15935,11 +15994,11 @@
       </c>
       <c r="AC46">
         <f>Notes!$C$7 * Notes!$K$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>197990400</v>
+        <v>27124684800</v>
       </c>
       <c r="AD46">
         <f>Notes!$D$7 * Notes!$L$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>8798285220</v>
       </c>
       <c r="AE46">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -16027,11 +16086,11 @@
       </c>
       <c r="AC47">
         <f>Notes!$C$7 * Notes!$K$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>197990400</v>
+        <v>27124684800</v>
       </c>
       <c r="AD47">
         <f>Notes!$D$7 * Notes!$L$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>8798285220</v>
       </c>
       <c r="AE47">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -16119,11 +16178,11 @@
       </c>
       <c r="AC48">
         <f>Notes!$C$7 * Notes!$K$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>197990400</v>
+        <v>27124684800</v>
       </c>
       <c r="AD48">
         <f>Notes!$D$7 * Notes!$L$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>8798285220</v>
       </c>
       <c r="AE48">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -16211,11 +16270,11 @@
       </c>
       <c r="AC49">
         <f>Notes!$C$7 * Notes!$K$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>197990400</v>
+        <v>27124684800</v>
       </c>
       <c r="AD49">
         <f>Notes!$D$7 * Notes!$L$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>8798285220</v>
       </c>
       <c r="AE49">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -16313,7 +16372,7 @@
       </c>
       <c r="AD50">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE50">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -16411,7 +16470,7 @@
       </c>
       <c r="AD51">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE51">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -16509,7 +16568,7 @@
       </c>
       <c r="AD52">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE52">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -16605,7 +16664,7 @@
       </c>
       <c r="AD53">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE53">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -16705,7 +16764,7 @@
       </c>
       <c r="AD54">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE54">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -16803,7 +16862,7 @@
       </c>
       <c r="AD55">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE55">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -16899,7 +16958,7 @@
       </c>
       <c r="AD56">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE56">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -16989,7 +17048,7 @@
       </c>
       <c r="AD57">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE57">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -17079,7 +17138,7 @@
       </c>
       <c r="AD58">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE58">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -17169,7 +17228,7 @@
       </c>
       <c r="AD59">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE59">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -17259,7 +17318,7 @@
       </c>
       <c r="AD60">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE60">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -17347,7 +17406,7 @@
       </c>
       <c r="AD61">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE61">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -17435,7 +17494,7 @@
       </c>
       <c r="AD62">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE62">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -17525,7 +17584,7 @@
       </c>
       <c r="AD63">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE63">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -17615,7 +17674,7 @@
       </c>
       <c r="AD64">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE64">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -17703,7 +17762,7 @@
       </c>
       <c r="AD65">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE65">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -17791,7 +17850,7 @@
       </c>
       <c r="AD66">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE66">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -17881,7 +17940,7 @@
       </c>
       <c r="AD67">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE67">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -17971,7 +18030,7 @@
       </c>
       <c r="AD68">
         <f>Notes!$D$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
-        <v>1140</v>
+        <v>1220200140</v>
       </c>
       <c r="AE68">
         <f>Notes!$E$7 * 19 * Notes!$C$10 * Notes!$C$13</f>
@@ -18059,7 +18118,7 @@
       </c>
       <c r="AD69">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE69">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -18147,7 +18206,7 @@
       </c>
       <c r="AD70">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE70">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -18235,7 +18294,7 @@
       </c>
       <c r="AD71">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE71">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -18323,7 +18382,7 @@
       </c>
       <c r="AD72">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE72">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -18411,7 +18470,7 @@
       </c>
       <c r="AD73">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE73">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -18499,7 +18558,7 @@
       </c>
       <c r="AD74">
         <f>Notes!$D$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>64221060</v>
       </c>
       <c r="AE74">
         <f>Notes!$E$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -18585,11 +18644,11 @@
       </c>
       <c r="AC75">
         <f>Notes!$C$7 * Notes!$K$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>197990400</v>
+        <v>27124684800</v>
       </c>
       <c r="AD75">
         <f>Notes!$D$7 * Notes!$L$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>8798285220</v>
       </c>
       <c r="AE75">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -18675,11 +18734,11 @@
       </c>
       <c r="AC76">
         <f>Notes!$C$7 * Notes!$K$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>197990400</v>
+        <v>27124684800</v>
       </c>
       <c r="AD76">
         <f>Notes!$D$7 * Notes!$L$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>8798285220</v>
       </c>
       <c r="AE76">
         <f>Notes!$E$7 * Notes!$M$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -18888,7 +18947,7 @@
       </c>
       <c r="AD2">
         <f>Notes!$H$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>12064160675</v>
       </c>
       <c r="AE2">
         <f>Notes!$I$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -18978,7 +19037,7 @@
       </c>
       <c r="AD3">
         <f>Notes!$H$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>12064160675</v>
       </c>
       <c r="AE3">
         <f>Notes!$I$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -19068,7 +19127,7 @@
       </c>
       <c r="AD4">
         <f>Notes!$H$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>12064160675</v>
       </c>
       <c r="AE4">
         <f>Notes!$I$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -19277,7 +19336,7 @@
       </c>
       <c r="AD2">
         <f>Notes!$H$7 * Notes!$C$13</f>
-        <v>5</v>
+        <v>33052495</v>
       </c>
       <c r="AE2">
         <f>Notes!$I$7 *  Notes!$C$13</f>
@@ -19365,7 +19424,7 @@
       </c>
       <c r="AD3">
         <f>Notes!$H$7 * Notes!$P$7 *  Notes!$C$13</f>
-        <v>5</v>
+        <v>2478937125</v>
       </c>
       <c r="AE3">
         <f>Notes!$I$7 * Notes!$Q$7 * Notes!$C$13</f>
@@ -19453,7 +19512,7 @@
       </c>
       <c r="AD4">
         <f>Notes!$H$7 * Notes!$C$13</f>
-        <v>5</v>
+        <v>33052495</v>
       </c>
       <c r="AE4">
         <f>Notes!$I$7 *  Notes!$C$13</f>
@@ -19543,7 +19602,7 @@
       </c>
       <c r="AD5">
         <f>Notes!$H$7 * Notes!$C$13</f>
-        <v>5</v>
+        <v>33052495</v>
       </c>
       <c r="AE5">
         <f>Notes!$I$7 *  Notes!$C$13</f>
@@ -19631,7 +19690,7 @@
       </c>
       <c r="AD6">
         <f>Notes!$H$7 * Notes!$C$13</f>
-        <v>5</v>
+        <v>33052495</v>
       </c>
       <c r="AE6">
         <f>Notes!$I$7 *  Notes!$C$13</f>
@@ -19721,7 +19780,7 @@
       </c>
       <c r="AD7">
         <f>Notes!$H$7 * Notes!$C$13</f>
-        <v>5</v>
+        <v>33052495</v>
       </c>
       <c r="AE7">
         <f>Notes!$I$7 *  Notes!$C$13</f>
@@ -19811,7 +19870,7 @@
       </c>
       <c r="AD8">
         <f>Notes!$H$7 * Notes!$P$7 *  Notes!$C$13</f>
-        <v>5</v>
+        <v>2478937125</v>
       </c>
       <c r="AE8">
         <f>Notes!$I$7 * Notes!$Q$7 * Notes!$C$13</f>
@@ -19899,7 +19958,7 @@
       </c>
       <c r="AD9">
         <f>Notes!$H$7 * Notes!$P$7 *  Notes!$C$13</f>
-        <v>5</v>
+        <v>2478937125</v>
       </c>
       <c r="AE9">
         <f>Notes!$I$7 * Notes!$Q$7 * Notes!$C$13</f>
@@ -19987,7 +20046,7 @@
       </c>
       <c r="AD10">
         <f>Notes!$H$7 * Notes!$C$13</f>
-        <v>5</v>
+        <v>33052495</v>
       </c>
       <c r="AE10">
         <f>Notes!$I$7 *  Notes!$C$13</f>
@@ -20204,7 +20263,7 @@
       </c>
       <c r="AD2">
         <f>Notes!$H$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>396629940</v>
       </c>
       <c r="AE2">
         <f>Notes!$I$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -20294,7 +20353,7 @@
       </c>
       <c r="AD3">
         <f>Notes!$H$7 * Notes!$P$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>29747245500</v>
       </c>
       <c r="AE3">
         <f>Notes!$I$7 * Notes!$Q$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -20394,7 +20453,7 @@
       </c>
       <c r="AD4">
         <f>Notes!$H$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>396629940</v>
       </c>
       <c r="AE4">
         <f>Notes!$I$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -20492,7 +20551,7 @@
       </c>
       <c r="AD5">
         <f>Notes!$H$7 * Notes!$P$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>29747245500</v>
       </c>
       <c r="AE5">
         <f>Notes!$I$7 * Notes!$Q$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -20590,7 +20649,7 @@
       </c>
       <c r="AD6">
         <f>Notes!$H$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>396629940</v>
       </c>
       <c r="AE6">
         <f>Notes!$I$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -20680,7 +20739,7 @@
       </c>
       <c r="AD7">
         <f>Notes!$H$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>396629940</v>
       </c>
       <c r="AE7">
         <f>Notes!$I$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -20770,7 +20829,7 @@
       </c>
       <c r="AD8">
         <f>Notes!$H$7 * Notes!$P$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>29747245500</v>
       </c>
       <c r="AE8">
         <f>Notes!$I$7 * Notes!$Q$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -20860,7 +20919,7 @@
       </c>
       <c r="AD9">
         <f>Notes!$H$7 * Notes!$P$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>29747245500</v>
       </c>
       <c r="AE9">
         <f>Notes!$I$7 * Notes!$Q$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -20948,7 +21007,7 @@
       </c>
       <c r="AD10">
         <f>Notes!$H$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>396629940</v>
       </c>
       <c r="AE10">
         <f>Notes!$I$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -21040,7 +21099,7 @@
       </c>
       <c r="AD11">
         <f>Notes!$H$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>396629940</v>
       </c>
       <c r="AE11">
         <f>Notes!$I$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -21130,7 +21189,7 @@
       </c>
       <c r="AD12">
         <f>Notes!$H$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>396629940</v>
       </c>
       <c r="AE12">
         <f>Notes!$I$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -21222,7 +21281,7 @@
       </c>
       <c r="AD13">
         <f>Notes!$H$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>396629940</v>
       </c>
       <c r="AE13">
         <f>Notes!$I$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -21314,7 +21373,7 @@
       </c>
       <c r="AD14">
         <f>Notes!$H$7 * Notes!$P$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>29747245500</v>
       </c>
       <c r="AE14">
         <f>Notes!$I$7 * Notes!$Q$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -21404,7 +21463,7 @@
       </c>
       <c r="AD15">
         <f>Notes!$H$7 * Notes!$P$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>29747245500</v>
       </c>
       <c r="AE15">
         <f>Notes!$I$7 * Notes!$Q$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -21496,7 +21555,7 @@
       </c>
       <c r="AD16">
         <f>Notes!$H$7 * Notes!$P$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>29747245500</v>
       </c>
       <c r="AE16">
         <f>Notes!$I$7 * Notes!$Q$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -21711,7 +21770,7 @@
       </c>
       <c r="AD2">
         <f>Notes!$H$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>12064160675</v>
       </c>
       <c r="AE2">
         <f>Notes!$I$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -21799,7 +21858,7 @@
       </c>
       <c r="AD3">
         <f>Notes!$D$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>1953390575</v>
       </c>
       <c r="AE3">
         <f>Notes!$E$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -21895,7 +21954,7 @@
       </c>
       <c r="AD4">
         <f>Notes!$H$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>12064160675</v>
       </c>
       <c r="AE4">
         <f>Notes!$I$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -21983,7 +22042,7 @@
       </c>
       <c r="AD5">
         <f>Notes!$H$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>12064160675</v>
       </c>
       <c r="AE5">
         <f>Notes!$I$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -22071,7 +22130,7 @@
       </c>
       <c r="AD6">
         <f>Notes!$H$7 * Notes!$D$10 * Notes!$C$13</f>
-        <v>1825</v>
+        <v>12064160675</v>
       </c>
       <c r="AE6">
         <f>Notes!$I$7 * Notes!$D$10 * Notes!$C$13</f>
@@ -22286,7 +22345,7 @@
       </c>
       <c r="AD2">
         <f>Notes!$H$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>396629940</v>
       </c>
       <c r="AE2">
         <f>Notes!$I$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -22374,7 +22433,7 @@
       </c>
       <c r="AD3">
         <f>Notes!$H$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>396629940</v>
       </c>
       <c r="AE3">
         <f>Notes!$I$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -22464,7 +22523,7 @@
       </c>
       <c r="AD4">
         <f>Notes!$H$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>396629940</v>
       </c>
       <c r="AE4">
         <f>Notes!$I$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -22554,7 +22613,7 @@
       </c>
       <c r="AD5">
         <f>Notes!$H$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>396629940</v>
       </c>
       <c r="AE5">
         <f>Notes!$I$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -22642,7 +22701,7 @@
       </c>
       <c r="AD6">
         <f>Notes!$H$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>396629940</v>
       </c>
       <c r="AE6">
         <f>Notes!$I$7 * Notes!$C$10 * Notes!$C$13</f>
@@ -22730,7 +22789,7 @@
       </c>
       <c r="AD7">
         <f>Notes!$H$7 * Notes!$C$10 * Notes!$C$13</f>
-        <v>60</v>
+        <v>396629940</v>
       </c>
       <c r="AE7">
         <f>Notes!$I$7 * Notes!$C$10 * Notes!$C$13</f>

</xml_diff>